<commit_message>
reorganize the provided designes in 2 files DES_LL & DES_HL
</commit_message>
<xml_diff>
--- a/Project Management/PM_Plan_BackLog.xlsx
+++ b/Project Management/PM_Plan_BackLog.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19140" windowHeight="7340"/>
   </bookViews>
   <sheets>
-    <sheet name="Time Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="TimePlan" sheetId="1" r:id="rId1"/>
     <sheet name="Effort Estimation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>Task Name</t>
   </si>
@@ -601,7 +601,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A13" sqref="A13:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,8 +802,8 @@
       <c r="H6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>46</v>
+      <c r="I6" s="15">
+        <v>3</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>20</v>
@@ -1008,7 +1008,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,7 +1046,7 @@
       <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       <c r="B4">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>7</v>
       </c>
     </row>

</xml_diff>